<commit_message>
default to WrapText = true
</commit_message>
<xml_diff>
--- a/src/Tests/EnumerableStringTests.Test.DotNet.verified.xlsx
+++ b/src/Tests/EnumerableStringTests.Test.DotNet.verified.xlsx
@@ -142,13 +142,9 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -474,7 +470,7 @@
       <x:c r="A2" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="s">
+      <x:c r="B2" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Revert "default to WrapText = true"
This reverts commit 5f3a70e9c86aba3336d9667c273f519a747c2a58.
</commit_message>
<xml_diff>
--- a/src/Tests/EnumerableStringTests.Test.DotNet.verified.xlsx
+++ b/src/Tests/EnumerableStringTests.Test.DotNet.verified.xlsx
@@ -142,9 +142,13 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -470,7 +474,7 @@
       <x:c r="A2" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B2" s="1" t="s">
+      <x:c r="B2" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>

</xml_diff>